<commit_message>
fixed issues restulted from extra files
</commit_message>
<xml_diff>
--- a/Data_preparation/datasets/final_data/21VIANET_GROUP_INC_ADR.xlsx
+++ b/Data_preparation/datasets/final_data/21VIANET_GROUP_INC_ADR.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="44">
   <si>
     <t>Ticker</t>
   </si>
@@ -146,117 +146,6 @@
   </si>
   <si>
     <t>USD</t>
-  </si>
-  <si>
-    <t>WIX</t>
-  </si>
-  <si>
-    <t>NOC</t>
-  </si>
-  <si>
-    <t>CDNS</t>
-  </si>
-  <si>
-    <t>NOW</t>
-  </si>
-  <si>
-    <t>NTAP</t>
-  </si>
-  <si>
-    <t>ROK</t>
-  </si>
-  <si>
-    <t>HPE</t>
-  </si>
-  <si>
-    <t>CYBR</t>
-  </si>
-  <si>
-    <t>ERIC</t>
-  </si>
-  <si>
-    <t>EBAY</t>
-  </si>
-  <si>
-    <t>FTNT</t>
-  </si>
-  <si>
-    <t>TSM</t>
-  </si>
-  <si>
-    <t>VRNT</t>
-  </si>
-  <si>
-    <t>INTC</t>
-  </si>
-  <si>
-    <t>TRI</t>
-  </si>
-  <si>
-    <t>OKTA</t>
-  </si>
-  <si>
-    <t>SNAP</t>
-  </si>
-  <si>
-    <t>MCHP</t>
-  </si>
-  <si>
-    <t>DOCU</t>
-  </si>
-  <si>
-    <t>UBER</t>
-  </si>
-  <si>
-    <t>ZBRA</t>
-  </si>
-  <si>
-    <t>ZS</t>
-  </si>
-  <si>
-    <t>NFLX</t>
-  </si>
-  <si>
-    <t>CSCO</t>
-  </si>
-  <si>
-    <t>AAPL</t>
-  </si>
-  <si>
-    <t>STNE</t>
-  </si>
-  <si>
-    <t>CAN</t>
-  </si>
-  <si>
-    <t>TSLA</t>
-  </si>
-  <si>
-    <t>DXC</t>
-  </si>
-  <si>
-    <t>UI</t>
-  </si>
-  <si>
-    <t>INFA</t>
-  </si>
-  <si>
-    <t>STX</t>
-  </si>
-  <si>
-    <t>FICO</t>
-  </si>
-  <si>
-    <t>AMBA</t>
-  </si>
-  <si>
-    <t>PEGA</t>
-  </si>
-  <si>
-    <t>PATH</t>
-  </si>
-  <si>
-    <t>AMZN</t>
   </si>
 </sst>
 </file>
@@ -763,22 +652,22 @@
         <v>42094</v>
       </c>
       <c r="D2">
-        <v>19.17000007629395</v>
+        <v>18.1299991607666</v>
       </c>
       <c r="E2">
-        <v>19.46999931335449</v>
+        <v>20.56999969482422</v>
       </c>
       <c r="F2">
-        <v>21.10000038146973</v>
+        <v>20.94000053405762</v>
       </c>
       <c r="G2">
-        <v>18.63999938964844</v>
+        <v>16.84000015258789</v>
       </c>
       <c r="H2">
-        <v>55686229</v>
+        <v>263895614</v>
       </c>
       <c r="I2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J2">
         <v>1166482899</v>
@@ -879,22 +768,22 @@
         <v>42185</v>
       </c>
       <c r="D3">
-        <v>135.1841268565159</v>
+        <v>20.54999923706055</v>
       </c>
       <c r="E3">
-        <v>146.5059204101562</v>
+        <v>20.26000022888184</v>
       </c>
       <c r="F3">
-        <v>149.4612783851101</v>
+        <v>21.02000045776367</v>
       </c>
       <c r="G3">
-        <v>133.8800511327204</v>
+        <v>15.02999973297119</v>
       </c>
       <c r="H3">
-        <v>143182982</v>
+        <v>263895614</v>
       </c>
       <c r="I3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J3">
         <v>1355392361</v>
@@ -995,22 +884,22 @@
         <v>42277</v>
       </c>
       <c r="D4">
-        <v>20.73999977111816</v>
+        <v>18.34000015258789</v>
       </c>
       <c r="E4">
-        <v>22.21999931335449</v>
+        <v>20.04000091552734</v>
       </c>
       <c r="F4">
-        <v>23.29999923706055</v>
+        <v>20.47999954223633</v>
       </c>
       <c r="G4">
-        <v>20.07999992370605</v>
+        <v>17.80999946594238</v>
       </c>
       <c r="H4">
-        <v>272490000</v>
+        <v>263895614</v>
       </c>
       <c r="I4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J4">
         <v>1207435300</v>
@@ -1111,22 +1000,22 @@
         <v>42369</v>
       </c>
       <c r="D5">
-        <v>84.98000335693359</v>
+        <v>20.59000015258789</v>
       </c>
       <c r="E5">
-        <v>62.20999908447266</v>
+        <v>19.19000053405762</v>
       </c>
       <c r="F5">
-        <v>85.66999816894531</v>
+        <v>20.88999938964844</v>
       </c>
       <c r="G5">
-        <v>57.66999816894531</v>
+        <v>18.22999954223633</v>
       </c>
       <c r="H5">
-        <v>207519000</v>
+        <v>263895614</v>
       </c>
       <c r="I5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="J5">
         <v>1396344762</v>
@@ -1227,22 +1116,22 @@
         <v>42460</v>
       </c>
       <c r="D6">
-        <v>21.06878244070543</v>
+        <v>19.80999946594238</v>
       </c>
       <c r="E6">
-        <v>18.4537239074707</v>
+        <v>20.18000030517578</v>
       </c>
       <c r="F6">
-        <v>21.22490591599555</v>
+        <v>21.1200008392334</v>
       </c>
       <c r="G6">
-        <v>18.25076398515507</v>
+        <v>19.63999938964844</v>
       </c>
       <c r="H6">
-        <v>199618386</v>
+        <v>263895614</v>
       </c>
       <c r="I6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J6">
         <v>1739443903</v>
@@ -1343,22 +1232,22 @@
         <v>42551</v>
       </c>
       <c r="D7">
-        <v>96.04321029982444</v>
+        <v>10.10000038146973</v>
       </c>
       <c r="E7">
-        <v>95.93419647216795</v>
+        <v>9.579999923706056</v>
       </c>
       <c r="F7">
-        <v>101.2592138942743</v>
+        <v>10.47999954223633</v>
       </c>
       <c r="G7">
-        <v>92.99075914643778</v>
+        <v>8.880000114440918</v>
       </c>
       <c r="H7">
-        <v>112434397</v>
+        <v>263895614</v>
       </c>
       <c r="I7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="J7">
         <v>889320093</v>
@@ -1459,22 +1348,22 @@
         <v>42643</v>
       </c>
       <c r="D8">
-        <v>10.08891169552178</v>
+        <v>7.909999847412109</v>
       </c>
       <c r="E8">
-        <v>10.03531837463379</v>
+        <v>7.309999942779541</v>
       </c>
       <c r="F8">
-        <v>10.24075858308116</v>
+        <v>8.079999923706055</v>
       </c>
       <c r="G8">
-        <v>9.423462821204105</v>
+        <v>6.769999980926514</v>
       </c>
       <c r="H8">
-        <v>1319450062</v>
+        <v>263895614</v>
       </c>
       <c r="I8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="J8">
         <v>692467653</v>
@@ -1575,22 +1464,22 @@
         <v>42735</v>
       </c>
       <c r="D9">
-        <v>45.97999954223633</v>
+        <v>7.059999942779541</v>
       </c>
       <c r="E9">
-        <v>53.06000137329102</v>
+        <v>7.170000076293945</v>
       </c>
       <c r="F9">
-        <v>53.20000076293945</v>
+        <v>7.550000190734863</v>
       </c>
       <c r="G9">
-        <v>45.61000061035156</v>
+        <v>6.960000038146973</v>
       </c>
       <c r="H9">
-        <v>50476952</v>
+        <v>263895614</v>
       </c>
       <c r="I9" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="J9">
         <v>610590974</v>
@@ -1691,22 +1580,22 @@
         <v>42825</v>
       </c>
       <c r="D10">
-        <v>5.311937668057123</v>
+        <v>5.480000019073486</v>
       </c>
       <c r="E10">
-        <v>5.160849571228027</v>
+        <v>5.409999847412109</v>
       </c>
       <c r="F10">
-        <v>5.327841658292762</v>
+        <v>5.710000038146973</v>
       </c>
       <c r="G10">
-        <v>4.930241523220734</v>
+        <v>5.28000020980835</v>
       </c>
       <c r="H10">
-        <v>3071530678</v>
+        <v>263895614</v>
       </c>
       <c r="I10" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="J10">
         <v>622194123</v>
@@ -1807,22 +1696,22 @@
         <v>42916</v>
       </c>
       <c r="D11">
-        <v>70.19999694824219</v>
+        <v>5.010000228881836</v>
       </c>
       <c r="E11">
-        <v>61.70000076293945</v>
+        <v>4.460000038146973</v>
       </c>
       <c r="F11">
-        <v>77.92500305175781</v>
+        <v>5.03000020980835</v>
       </c>
       <c r="G11">
-        <v>61</v>
+        <v>4.300000190734863</v>
       </c>
       <c r="H11">
-        <v>55686229</v>
+        <v>263895614</v>
       </c>
       <c r="I11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J11">
         <v>568927960</v>
@@ -1923,22 +1812,22 @@
         <v>43008</v>
       </c>
       <c r="D12">
-        <v>34.39338093652559</v>
+        <v>5.71999979019165</v>
       </c>
       <c r="E12">
-        <v>33.61638259887695</v>
+        <v>7.510000228881836</v>
       </c>
       <c r="F12">
-        <v>35.08107037354011</v>
+        <v>7.940000057220459</v>
       </c>
       <c r="G12">
-        <v>32.32138309818511</v>
+        <v>5.659999847412109</v>
       </c>
       <c r="H12">
-        <v>457000000</v>
+        <v>263895614</v>
       </c>
       <c r="I12" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="J12">
         <v>644860576</v>
@@ -2039,22 +1928,22 @@
         <v>43100</v>
       </c>
       <c r="D13">
-        <v>8.751999855041504</v>
+        <v>8.109999656677246</v>
       </c>
       <c r="E13">
-        <v>9.208000183105469</v>
+        <v>9.109999656677246</v>
       </c>
       <c r="F13">
-        <v>9.28600025177002</v>
+        <v>9.590000152587891</v>
       </c>
       <c r="G13">
-        <v>8.696000099182129</v>
+        <v>7.96999979019165</v>
       </c>
       <c r="H13">
-        <v>766266033</v>
+        <v>263895614</v>
       </c>
       <c r="I13" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="J13">
         <v>904391458</v>
@@ -2155,22 +2044,22 @@
         <v>43190</v>
       </c>
       <c r="D14">
-        <v>35.97240561616163</v>
+        <v>6.920000076293945</v>
       </c>
       <c r="E14">
-        <v>31.91368293762207</v>
+        <v>5.269999980926514</v>
       </c>
       <c r="F14">
-        <v>36.75260893317965</v>
+        <v>7.179999828338623</v>
       </c>
       <c r="G14">
-        <v>31.53188151649943</v>
+        <v>5.110000133514404</v>
       </c>
       <c r="H14">
-        <v>5186523104</v>
+        <v>263895614</v>
       </c>
       <c r="I14" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="J14">
         <v>775490127</v>
@@ -2271,22 +2160,22 @@
         <v>43281</v>
       </c>
       <c r="D15">
-        <v>22.36372947692871</v>
+        <v>9.640000343322754</v>
       </c>
       <c r="E15">
-        <v>22.87315368652344</v>
+        <v>9.439999580383301</v>
       </c>
       <c r="F15">
-        <v>25.01273536682129</v>
+        <v>11.53999996185303</v>
       </c>
       <c r="G15">
-        <v>22.00713157653809</v>
+        <v>8.399999618530273</v>
       </c>
       <c r="H15">
-        <v>60308678</v>
+        <v>263895614</v>
       </c>
       <c r="I15" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="J15">
         <v>1085462371</v>
@@ -2387,22 +2276,22 @@
         <v>43373</v>
       </c>
       <c r="D16">
-        <v>40.01662959399956</v>
+        <v>10.11999988555908</v>
       </c>
       <c r="E16">
-        <v>40.09360122680664</v>
+        <v>10.88000011444092</v>
       </c>
       <c r="F16">
-        <v>42.52247987457982</v>
+        <v>11.47999954223633</v>
       </c>
       <c r="G16">
-        <v>36.22792094161961</v>
+        <v>9.229999542236328</v>
       </c>
       <c r="H16">
-        <v>4757218036</v>
+        <v>263895614</v>
       </c>
       <c r="I16" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="J16">
         <v>1130223706</v>
@@ -2503,22 +2392,22 @@
         <v>43465</v>
       </c>
       <c r="D17">
-        <v>42.82212632249508</v>
+        <v>8.510000228881836</v>
       </c>
       <c r="E17">
-        <v>46.75239944458008</v>
+        <v>8.979999542236328</v>
       </c>
       <c r="F17">
-        <v>46.95784665825049</v>
+        <v>9.770000457763672</v>
       </c>
       <c r="G17">
-        <v>41.83955640128374</v>
+        <v>8.239999771118164</v>
       </c>
       <c r="H17">
-        <v>450687724</v>
+        <v>263895614</v>
       </c>
       <c r="I17" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="J17">
         <v>966844833</v>
@@ -2619,22 +2508,22 @@
         <v>43555</v>
       </c>
       <c r="D18">
-        <v>83.62000274658203</v>
+        <v>8</v>
       </c>
       <c r="E18">
-        <v>104.0299987792969</v>
+        <v>7.860000133514404</v>
       </c>
       <c r="F18">
-        <v>104.9800033569336</v>
+        <v>8.229999542236328</v>
       </c>
       <c r="G18">
-        <v>82.03099822998047</v>
+        <v>7</v>
       </c>
       <c r="H18">
-        <v>168459019</v>
+        <v>263895614</v>
       </c>
       <c r="I18" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="J18">
         <v>892576605</v>
@@ -2747,22 +2636,22 @@
         <v>43646</v>
       </c>
       <c r="D19">
-        <v>14.72999954223633</v>
+        <v>7.880000114440918</v>
       </c>
       <c r="E19">
-        <v>16.79999923706055</v>
+        <v>7.360000133514404</v>
       </c>
       <c r="F19">
-        <v>18.36000061035156</v>
+        <v>8.119999885559082</v>
       </c>
       <c r="G19">
-        <v>13.96000003814697</v>
+        <v>7</v>
       </c>
       <c r="H19">
-        <v>1435682333</v>
+        <v>263895614</v>
       </c>
       <c r="I19" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="J19">
         <v>875714327</v>
@@ -2863,22 +2752,22 @@
         <v>43738</v>
       </c>
       <c r="D20">
-        <v>42.51583583355016</v>
+        <v>7.590000152587891</v>
       </c>
       <c r="E20">
-        <v>42.25590896606445</v>
+        <v>8.479999542236328</v>
       </c>
       <c r="F20">
-        <v>43.8557984628152</v>
+        <v>8.800000190734863</v>
       </c>
       <c r="G20">
-        <v>39.92553545962458</v>
+        <v>7.119999885559082</v>
       </c>
       <c r="H20">
-        <v>539679667</v>
+        <v>263895614</v>
       </c>
       <c r="I20" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="J20">
         <v>856603744</v>
@@ -2979,22 +2868,22 @@
         <v>43830</v>
       </c>
       <c r="D21">
-        <v>74.30999755859375</v>
+        <v>7.489999771118164</v>
       </c>
       <c r="E21">
-        <v>78.51000213623047</v>
+        <v>9.239999771118164</v>
       </c>
       <c r="F21">
-        <v>80.26000213623047</v>
+        <v>11.25</v>
       </c>
       <c r="G21">
-        <v>70.55000305175781</v>
+        <v>7.260000228881836</v>
       </c>
       <c r="H21">
-        <v>201104117</v>
+        <v>263895614</v>
       </c>
       <c r="I21" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="J21">
         <v>815010124</v>
@@ -3095,22 +2984,22 @@
         <v>43921</v>
       </c>
       <c r="D22">
-        <v>26.5</v>
+        <v>13.35000038146973</v>
       </c>
       <c r="E22">
-        <v>30.27000045776367</v>
+        <v>14.97000026702881</v>
       </c>
       <c r="F22">
-        <v>32</v>
+        <v>17.3700008392334</v>
       </c>
       <c r="G22">
-        <v>21.67000007629395</v>
+        <v>12.71000003814697</v>
       </c>
       <c r="H22">
-        <v>2085418676</v>
+        <v>263895614</v>
       </c>
       <c r="I22" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="J22">
         <v>1571029800</v>
@@ -3211,22 +3100,22 @@
         <v>44012</v>
       </c>
       <c r="D23">
-        <v>256.4700012207031</v>
+        <v>24</v>
       </c>
       <c r="E23">
-        <v>280.75</v>
+        <v>21.73999977111816</v>
       </c>
       <c r="F23">
-        <v>287.8299865722656</v>
+        <v>30.44000053405762</v>
       </c>
       <c r="G23">
-        <v>250.9499969482422</v>
+        <v>21.04999923706055</v>
       </c>
       <c r="H23">
-        <v>50845151</v>
+        <v>263895614</v>
       </c>
       <c r="I23" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="J23">
         <v>2704528935</v>
@@ -3327,22 +3216,22 @@
         <v>44104</v>
       </c>
       <c r="D24">
-        <v>142.1999969482422</v>
+        <v>23.51000022888184</v>
       </c>
       <c r="E24">
-        <v>135.75</v>
+        <v>22.95999908447266</v>
       </c>
       <c r="F24">
-        <v>158.7359924316406</v>
+        <v>26.57999992370605</v>
       </c>
       <c r="G24">
-        <v>133.8099975585938</v>
+        <v>21.5</v>
       </c>
       <c r="H24">
-        <v>158300823</v>
+        <v>263895614</v>
       </c>
       <c r="I24" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="J24">
         <v>2625183995</v>
@@ -3443,22 +3332,22 @@
         <v>44196</v>
       </c>
       <c r="D25">
-        <v>29.91399955749512</v>
+        <v>35</v>
       </c>
       <c r="E25">
-        <v>28.95000076293945</v>
+        <v>37.72999954223633</v>
       </c>
       <c r="F25">
-        <v>31.0620002746582</v>
+        <v>43.79999923706055</v>
       </c>
       <c r="G25">
-        <v>27.46199989318848</v>
+        <v>32.09000015258789</v>
       </c>
       <c r="H25">
-        <v>766266033</v>
+        <v>263895614</v>
       </c>
       <c r="I25" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="J25">
         <v>3932108498</v>
@@ -3559,22 +3448,22 @@
         <v>44286</v>
       </c>
       <c r="D26">
-        <v>529.9299926757812</v>
+        <v>33.52000045776367</v>
       </c>
       <c r="E26">
-        <v>513.469970703125</v>
+        <v>27.90999984741211</v>
       </c>
       <c r="F26">
-        <v>563.5599975585938</v>
+        <v>34.88000106811523</v>
       </c>
       <c r="G26">
-        <v>499</v>
+        <v>26.80999946594238</v>
       </c>
       <c r="H26">
-        <v>424926346</v>
+        <v>263895614</v>
       </c>
       <c r="I26" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="J26">
         <v>4404230458</v>
@@ -3675,22 +3564,22 @@
         <v>44377</v>
       </c>
       <c r="D27">
-        <v>46.47724219552952</v>
+        <v>22.75</v>
       </c>
       <c r="E27">
-        <v>48.50979995727539</v>
+        <v>17.32999992370605</v>
       </c>
       <c r="F27">
-        <v>48.75511095753174</v>
+        <v>22.94000053405762</v>
       </c>
       <c r="G27">
-        <v>45.85521015250949</v>
+        <v>14.10999965667725</v>
       </c>
       <c r="H27">
-        <v>3953196953</v>
+        <v>263895614</v>
       </c>
       <c r="I27" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="J27">
         <v>3129321641</v>
@@ -3791,22 +3680,22 @@
         <v>44469</v>
       </c>
       <c r="D28">
-        <v>138.916410444292</v>
+        <v>17.18000030517578</v>
       </c>
       <c r="E28">
-        <v>146.6503143310547</v>
+        <v>15.68000030517578</v>
       </c>
       <c r="F28">
-        <v>149.9494520691154</v>
+        <v>19.65999984741211</v>
       </c>
       <c r="G28">
-        <v>135.3627448332334</v>
+        <v>15.3100004196167</v>
       </c>
       <c r="H28">
-        <v>14840390000</v>
+        <v>263895614</v>
       </c>
       <c r="I28" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="J28">
         <v>2522092540</v>
@@ -3910,22 +3799,22 @@
         <v>44561</v>
       </c>
       <c r="D29">
-        <v>17.05999946594238</v>
+        <v>9.149999618530272</v>
       </c>
       <c r="E29">
-        <v>15.57999992370606</v>
+        <v>9.920000076293944</v>
       </c>
       <c r="F29">
-        <v>19.65999984741211</v>
+        <v>10.28999996185303</v>
       </c>
       <c r="G29">
-        <v>13.14000034332275</v>
+        <v>7.730000019073486</v>
       </c>
       <c r="H29">
-        <v>250599325</v>
+        <v>263895614</v>
       </c>
       <c r="I29" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="J29">
         <v>1300043664</v>
@@ -4026,22 +3915,22 @@
         <v>44651</v>
       </c>
       <c r="D30">
-        <v>151.2200012207031</v>
+        <v>6.440000057220459</v>
       </c>
       <c r="E30">
-        <v>119.3099975585938</v>
+        <v>5.96999979019165</v>
       </c>
       <c r="F30">
-        <v>161.6100006103516</v>
+        <v>7.28000020980835</v>
       </c>
       <c r="G30">
-        <v>118.879997253418</v>
+        <v>5.079999923706055</v>
       </c>
       <c r="H30">
-        <v>168459019</v>
+        <v>263895614</v>
       </c>
       <c r="I30" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="J30">
         <v>839341590</v>
@@ -4142,22 +4031,22 @@
         <v>44742</v>
       </c>
       <c r="D31">
-        <v>3.200000047683716</v>
+        <v>5.96999979019165</v>
       </c>
       <c r="E31">
-        <v>3.930000066757202</v>
+        <v>5.159999847412109</v>
       </c>
       <c r="F31">
-        <v>4.539999961853027</v>
+        <v>6.28000020980835</v>
       </c>
       <c r="G31">
-        <v>3.109999895095825</v>
+        <v>4.610000133514404</v>
       </c>
       <c r="H31">
-        <v>448228270</v>
+        <v>263895614</v>
       </c>
       <c r="I31" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="J31">
         <v>894240897</v>
@@ -4258,22 +4147,22 @@
         <v>44834</v>
       </c>
       <c r="D32">
-        <v>254.5</v>
+        <v>5.550000190734863</v>
       </c>
       <c r="E32">
-        <v>227.5399932861328</v>
+        <v>4.190000057220459</v>
       </c>
       <c r="F32">
-        <v>257.5</v>
+        <v>6.019999980926514</v>
       </c>
       <c r="G32">
-        <v>198.5899963378907</v>
+        <v>4.070000171661377</v>
       </c>
       <c r="H32">
-        <v>3325150886</v>
+        <v>263895614</v>
       </c>
       <c r="I32" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="J32">
         <v>814292208</v>
@@ -4374,22 +4263,22 @@
         <v>44926</v>
       </c>
       <c r="D33">
-        <v>26.71999931335449</v>
+        <v>5.699999809265137</v>
       </c>
       <c r="E33">
-        <v>28.72999954223633</v>
+        <v>5.880000114440918</v>
       </c>
       <c r="F33">
-        <v>29.72999954223633</v>
+        <v>6.829999923706055</v>
       </c>
       <c r="G33">
-        <v>26.64999961853028</v>
+        <v>5.699999809265137</v>
       </c>
       <c r="H33">
-        <v>178998669</v>
+        <v>263895614</v>
       </c>
       <c r="I33" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="J33">
         <v>839461240</v>
@@ -4490,22 +4379,22 @@
         <v>45016</v>
       </c>
       <c r="D34">
-        <v>261.1884929516806</v>
+        <v>3.740000009536743</v>
       </c>
       <c r="E34">
-        <v>225.4617156982422</v>
+        <v>2.940000057220459</v>
       </c>
       <c r="F34">
-        <v>262.5264343168398</v>
+        <v>4.190000057220459</v>
       </c>
       <c r="G34">
-        <v>223.9783523558658</v>
+        <v>2.75</v>
       </c>
       <c r="H34">
-        <v>60498713</v>
+        <v>263895614</v>
       </c>
       <c r="I34" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="J34">
         <v>481081782</v>
@@ -4618,22 +4507,22 @@
         <v>45107</v>
       </c>
       <c r="D35">
-        <v>18.42000007629395</v>
+        <v>2.940000057220459</v>
       </c>
       <c r="E35">
-        <v>19.04000091552734</v>
+        <v>2.970000028610229</v>
       </c>
       <c r="F35">
-        <v>19.38999938964844</v>
+        <v>3.059999942779541</v>
       </c>
       <c r="G35">
-        <v>17.57999992370605</v>
+        <v>2.539999961853028</v>
       </c>
       <c r="H35">
-        <v>260676335</v>
+        <v>263895614</v>
       </c>
       <c r="I35" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="J35">
         <v>429471110</v>
@@ -4734,22 +4623,22 @@
         <v>45199</v>
       </c>
       <c r="D36">
-        <v>62.6169871617784</v>
+        <v>3.099999904632568</v>
       </c>
       <c r="E36">
-        <v>64.67326354980469</v>
+        <v>3.220000028610229</v>
       </c>
       <c r="F36">
-        <v>66.63478202323152</v>
+        <v>3.359999895095825</v>
       </c>
       <c r="G36">
-        <v>60.75970456328059</v>
+        <v>2.650000095367432</v>
       </c>
       <c r="H36">
-        <v>212968277</v>
+        <v>263895614</v>
       </c>
       <c r="I36" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="J36">
         <v>463701008</v>
@@ -4850,22 +4739,22 @@
         <v>45291</v>
       </c>
       <c r="D37">
-        <v>1152.400024414062</v>
+        <v>2.880000114440918</v>
       </c>
       <c r="E37">
-        <v>1198.829956054688</v>
+        <v>1.700000047683716</v>
       </c>
       <c r="F37">
-        <v>1307.140014648438</v>
+        <v>2.880000114440918</v>
       </c>
       <c r="G37">
-        <v>1113.18994140625</v>
+        <v>1.629999995231628</v>
       </c>
       <c r="H37">
-        <v>24003656</v>
+        <v>263895614</v>
       </c>
       <c r="I37" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="J37">
         <v>425351547</v>
@@ -4966,22 +4855,22 @@
         <v>45382</v>
       </c>
       <c r="D38">
-        <v>104.6600036621094</v>
+        <v>1.549999952316284</v>
       </c>
       <c r="E38">
-        <v>92.98000335693359</v>
+        <v>1.690000057220459</v>
       </c>
       <c r="F38">
-        <v>105.0100021362305</v>
+        <v>1.899999976158142</v>
       </c>
       <c r="G38">
-        <v>90.66999816894533</v>
+        <v>1.419999957084656</v>
       </c>
       <c r="H38">
-        <v>168459019</v>
+        <v>263895614</v>
       </c>
       <c r="I38" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="J38">
         <v>391093935</v>
@@ -5082,22 +4971,22 @@
         <v>45473</v>
       </c>
       <c r="D39">
-        <v>53.97000122070312</v>
+        <v>2.109999895095825</v>
       </c>
       <c r="E39">
-        <v>52.63999938964844</v>
+        <v>2.069999933242798</v>
       </c>
       <c r="F39">
-        <v>65.87999725341797</v>
+        <v>2.470000028610229</v>
       </c>
       <c r="G39">
-        <v>50.29000091552734</v>
+        <v>1.840000033378601</v>
       </c>
       <c r="H39">
-        <v>42689006</v>
+        <v>263895614</v>
       </c>
       <c r="I39" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="J39">
         <v>547707729</v>
@@ -5198,22 +5087,22 @@
         <v>45565</v>
       </c>
       <c r="D40">
-        <v>36.50313191135645</v>
+        <v>4.139999866485596</v>
       </c>
       <c r="E40">
-        <v>39.63111877441406</v>
+        <v>3.279999971389771</v>
       </c>
       <c r="F40">
-        <v>41.15769383693995</v>
+        <v>4.5</v>
       </c>
       <c r="G40">
-        <v>34.26814654717644</v>
+        <v>3.170000076293945</v>
       </c>
       <c r="H40">
-        <v>171080665</v>
+        <v>263895614</v>
       </c>
       <c r="I40" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="J40">
         <v>1084587101</v>
@@ -5314,22 +5203,22 @@
         <v>45657</v>
       </c>
       <c r="D41">
-        <v>12.96000003814697</v>
+        <v>4.760000228881836</v>
       </c>
       <c r="E41">
-        <v>14.22000026702881</v>
+        <v>6.96999979019165</v>
       </c>
       <c r="F41">
-        <v>15.34500026702881</v>
+        <v>8.140000343322754</v>
       </c>
       <c r="G41">
-        <v>12.61999988555908</v>
+        <v>4.610000133514404</v>
       </c>
       <c r="H41">
-        <v>453568899</v>
+        <v>263895614</v>
       </c>
       <c r="I41" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="J41">
         <v>1266512988</v>
@@ -5430,22 +5319,22 @@
         <v>45747</v>
       </c>
       <c r="D42">
-        <v>187.8600006103516</v>
+        <v>8.069999694824219</v>
       </c>
       <c r="E42">
-        <v>184.4199981689453</v>
+        <v>6.289999961853027</v>
       </c>
       <c r="F42">
-        <v>198.3399963378907</v>
+        <v>8.229999542236328</v>
       </c>
       <c r="G42">
-        <v>161.3800048828125</v>
+        <v>4.650000095367432</v>
       </c>
       <c r="H42">
-        <v>10664912097</v>
+        <v>263895614</v>
       </c>
       <c r="I42" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="J42">
         <v>2198438486</v>
@@ -5540,22 +5429,22 @@
         <v>45838</v>
       </c>
       <c r="D43">
-        <v>105.0804770925983</v>
+        <v>6.849999904632568</v>
       </c>
       <c r="E43">
-        <v>103.1780242919922</v>
+        <v>8.310000419616699</v>
       </c>
       <c r="F43">
-        <v>109.3114367486601</v>
+        <v>9.420000076293944</v>
       </c>
       <c r="G43">
-        <v>101.4440230697358</v>
+        <v>6.409999847412109</v>
       </c>
       <c r="H43">
-        <v>199618386</v>
+        <v>263895614</v>
       </c>
       <c r="I43" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J43">
         <v>1850489842</v>

</xml_diff>